<commit_message>
Add a sql sheet.
</commit_message>
<xml_diff>
--- a/image/c/data-foamt.xlsx
+++ b/image/c/data-foamt.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4755"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="sql" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="55">
   <si>
     <t>หนังสือเรียนรู้เพิ่มเติมเพื่อเสริมศักยภาพ ฟิสิกส์ เล่ม 1</t>
   </si>
@@ -180,6 +181,15 @@
   </si>
   <si>
     <t>หนังสือเรียนรู้เพิ่มเติมเพื่อเสริมศักยภาพ เวกเตอร์ในสามมิติ</t>
+  </si>
+  <si>
+    <t>INSERT INTO `ipst`.`book_category` (`id`, `name`) VALUES ("</t>
+  </si>
+  <si>
+    <t>", "</t>
+  </si>
+  <si>
+    <t>")</t>
   </si>
 </sst>
 </file>
@@ -251,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -259,6 +269,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,4 +974,876 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="52.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" customWidth="1"/>
+    <col min="4" max="4" width="75.5703125" customWidth="1"/>
+    <col min="5" max="5" width="3.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="7">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="7">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="7">
+        <v>3</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="7">
+        <v>4</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="7">
+        <v>5</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="7">
+        <v>6</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="7">
+        <v>7</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="7">
+        <v>8</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="7">
+        <v>9</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="7">
+        <v>10</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="7">
+        <v>11</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="7">
+        <v>12</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="7">
+        <v>13</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="7">
+        <v>14</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="7">
+        <v>15</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="7">
+        <v>16</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="7">
+        <v>17</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="7">
+        <v>18</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="7">
+        <v>19</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="7">
+        <v>20</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="7">
+        <v>21</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="7">
+        <v>22</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="7">
+        <v>23</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="7">
+        <v>24</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="7">
+        <v>25</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="7">
+        <v>26</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="7">
+        <v>27</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="7">
+        <v>28</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="7">
+        <v>29</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="7">
+        <v>30</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="7">
+        <v>31</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="7">
+        <v>32</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="7">
+        <v>33</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="7">
+        <v>34</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="7">
+        <v>35</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="7">
+        <v>36</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="7">
+        <v>37</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="7">
+        <v>38</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" s="7">
+        <v>39</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" s="7">
+        <v>40</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="7">
+        <v>41</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" s="7">
+        <v>42</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" s="7">
+        <v>43</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" s="7">
+        <v>44</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" s="7">
+        <v>45</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" s="7">
+        <v>46</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" s="7">
+        <v>47</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48" s="7">
+        <v>48</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="7">
+        <v>49</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" s="7">
+        <v>50</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Contribute book has been developed completely.
</commit_message>
<xml_diff>
--- a/image/c/data-foamt.xlsx
+++ b/image/c/data-foamt.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\ipst\image\c\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4755"/>
   </bookViews>
@@ -15,7 +10,7 @@
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="sql" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="61">
   <si>
     <t>หนังสือเรียนรู้เพิ่มเติมเพื่อเสริมศักยภาพ ฟิสิกส์ เล่ม 1</t>
   </si>
@@ -190,6 +185,24 @@
   </si>
   <si>
     <t>")</t>
+  </si>
+  <si>
+    <t>วีดิทัศน์ (DVD) ประกอบการเรียนรู้วิชาคณิตศาสตร์  ชั้นประถมศึกษาปีที่ 1</t>
+  </si>
+  <si>
+    <t>วีดิทัศน์ (DVD) ประกอบการเรียนรู้วิชาคณิตศาสตร์  ชั้นประถมศึกษาปีที่ 2</t>
+  </si>
+  <si>
+    <t>วีดิทัศน์ (DVD) ประกอบการเรียนรู้วิชาคณิตศาสตร์  ชั้นประถมศึกษาปีที่ 3</t>
+  </si>
+  <si>
+    <t>วีดิทัศน์ (DVD) ประกอบการเรียนรู้วิชาคณิตศาสตร์  ชั้นประถมศึกษาปีที่ 4</t>
+  </si>
+  <si>
+    <t>วีดิทัศน์ (DVD) ประกอบการเรียนรู้วิชาคณิตศาสตร์  ชั้นประถมศึกษาปีที่ 5</t>
+  </si>
+  <si>
+    <t>วีดิทัศน์ (DVD) ประกอบการเรียนรู้วิชาคณิตศาสตร์  ชั้นประถมศึกษาปีที่ 6</t>
   </si>
 </sst>
 </file>
@@ -543,7 +556,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -551,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,6 +981,54 @@
       </c>
       <c r="B51" s="4">
         <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" s="2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B54" s="2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" s="2">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>